<commit_message>
Upload of Completed Files
</commit_message>
<xml_diff>
--- a/Excel Test .xlsx
+++ b/Excel Test .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="120" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Answer Key" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Event data'!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -698,6 +698,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -725,7 +726,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1071,34 +1071,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
@@ -1139,7 +1139,7 @@
       <c r="A12" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="7">
         <f>INDEX('Event data'!E:E,MATCH(2003610,'Event data'!A:A,0))</f>
         <v>40727</v>
       </c>

</xml_diff>